<commit_message>
integrating frontend  login with backend api
</commit_message>
<xml_diff>
--- a/ReportsAndDocuments/worklog.xlsx
+++ b/ReportsAndDocuments/worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\300392759\Desktop\Dev\W26_4495_S3_ManeeshaE\ReportsAndDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6077B8DB-DE56-49FA-A7BF-D0780B2E80E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9BBA88-65C8-4FDB-8F99-B756F90EBCDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>fixed alignment issues of all interfaces,finaly found root cause in auth.css file which had default paddings and configurations,updated login and registration with 2 panel interface</t>
+  </si>
+  <si>
+    <t>in the process of connecting frontend with backend;</t>
+  </si>
+  <si>
+    <t>created SQL Server LocalDB database  in college pc by using migration files</t>
   </si>
 </sst>
 </file>
@@ -977,10 +983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE14CD6-E8F7-4785-AF16-07A58E8D9E8B}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,6 +1323,14 @@
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="24">
         <v>46065</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="26" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add updated issues doc, worklog, and SQL query
</commit_message>
<xml_diff>
--- a/ReportsAndDocuments/worklog.xlsx
+++ b/ReportsAndDocuments/worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\300392759\Desktop\Dev\W26_4495_S3_ManeeshaE\ReportsAndDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9A135F-DA33-49A6-A2CB-63825E809AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE0DF9D-D262-412D-8CBF-2660DC451E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>in the process of connecting frontend with backend;frontend login connected with backend login</t>
+  </si>
+  <si>
+    <t>resolving vite not loading environment error</t>
+  </si>
+  <si>
+    <t>resolving registering and login user issue</t>
+  </si>
+  <si>
+    <t>frontend user registration issue sorted : register page used mock mode and pointed to old url</t>
   </si>
 </sst>
 </file>
@@ -290,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -326,39 +335,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -369,6 +345,43 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,8 +698,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="225.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -765,9 +778,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
@@ -861,8 +874,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="9" t="s">
         <v>20</v>
       </c>
@@ -879,8 +892,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
@@ -908,8 +921,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="9" t="s">
         <v>25</v>
       </c>
@@ -948,41 +961,35 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="20"/>
       <c r="C35" s="9" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A22:A23"/>
@@ -991,6 +998,12 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -999,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE14CD6-E8F7-4785-AF16-07A58E8D9E8B}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,8 +1048,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="18"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="22"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1115,9 +1128,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="23"/>
+      <c r="A13" s="18"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
@@ -1211,8 +1224,8 @@
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18"/>
-      <c r="B23" s="16"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="20"/>
       <c r="C23" s="9" t="s">
         <v>20</v>
       </c>
@@ -1229,8 +1242,8 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="16"/>
+      <c r="A25" s="27"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="9" t="s">
         <v>22</v>
       </c>
@@ -1258,8 +1271,8 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="18"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="20"/>
       <c r="C28" s="9" t="s">
         <v>25</v>
       </c>
@@ -1298,68 +1311,86 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="15"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="15"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="24">
+      <c r="A36" s="13">
         <v>46063</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="14">
         <v>3</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="24">
+      <c r="A37" s="13">
         <v>46065</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="26" t="s">
+      <c r="B37" s="16"/>
+      <c r="C37" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="26" t="s">
+      <c r="A38" s="16"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="15" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="28">
+        <v>46068</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="28">
+        <v>46070</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A22:A23"/>
@@ -1368,6 +1399,12 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update db with MVP
</commit_message>
<xml_diff>
--- a/ReportsAndDocuments/worklog.xlsx
+++ b/ReportsAndDocuments/worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\300392759\Desktop\Dev\W26_4495_S3_ManeeshaE\ReportsAndDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB0367A-38B0-4F8A-9278-4EEBE7C1FAEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC1CED0-1233-4160-A914-F10F610F6069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -155,6 +155,9 @@
 DB persistence
 JWT working
 Protected routing</t>
+  </si>
+  <si>
+    <t>issues:table RelationshipStats has two foreign keys to the same table and sql server blocking that activity;solution : in AppDbContext.cs, add OnModelCreating and change delete behavior to Restriction for AT LEAST 1 FK</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE14CD6-E8F7-4785-AF16-07A58E8D9E8B}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,6 +1407,11 @@
     <row r="42" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="C42" s="30" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C44" s="29" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import API_BASE  from .env file
</commit_message>
<xml_diff>
--- a/ReportsAndDocuments/worklog.xlsx
+++ b/ReportsAndDocuments/worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\300392759\Desktop\Dev\W26_4495_S3_ManeeshaE\ReportsAndDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21EF5D8-F1DE-46E5-9BC5-9EBA40A92F12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B065C89-E834-4DEF-A22A-7681B7105BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>created Real DB data in dashboards</t>
+  </si>
+  <si>
+    <t>Updated FarmerDashboard with real data from DB</t>
   </si>
 </sst>
 </file>
@@ -1057,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE14CD6-E8F7-4785-AF16-07A58E8D9E8B}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,6 +1460,11 @@
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>